<commit_message>
Handle Surrogates If Read
It is probably very anal of me to do this. Excel does it. I can't see it happening in the wild.
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/issue.4724.xlsx
+++ b/tests/data/Reader/XLSX/issue.4724.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\issue4724\tests\data\Reader\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E9F953-1ED3-4AD1-9530-40B3E91C53F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D576FA4-9417-4F2B-84E6-84FF334ED61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>line_x000D_
 with_x000D_
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>_xC1EF_</t>
+  </si>
+  <si>
+    <t>_xD801__xDC05_</t>
+  </si>
+  <si>
+    <t>_xD801__x0038_</t>
+  </si>
+  <si>
+    <t>_x0039__xDC05_</t>
   </si>
 </sst>
 </file>
@@ -373,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -401,6 +410,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>